<commit_message>
add bib short title to table
</commit_message>
<xml_diff>
--- a/analyses/02_Literature/data/230220_Kidney_Genes_Publication_List.xlsx
+++ b/analyses/02_Literature/data/230220_Kidney_Genes_Publication_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fc256ff6cafd079a/!projekte/Nephrologie/Berlin/kidney-genetics/analyses/02_Literature/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\kidney-genetics\analyses\02_Literature\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{4C173233-A2B1-466B-9237-EFA0000D5C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3266A81-4FA1-49B0-B9BB-C6D14E794A30}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C49FC6-8328-47F2-86CD-9F06D89598EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-255" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Publications" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="133">
   <si>
     <t>Kidney Gene List (KG)</t>
   </si>
@@ -379,6 +379,57 @@
   </si>
   <si>
     <t>https://oup.silverchair-cdn.com/oup/backfile/Content_public/Journal/ndt/37/4/10.1093_ndt_gfab019/1/gfab019_supplementary_data.docx?Expires=1694696623&amp;Signature=gVIxow0K4oeDOWeVVjpH124MkvnKbbU5GSjCHQOFPwE1NvmkiSSWbGevW-zFni8kNHLU6hOlFIuiEszjh7bgZM1R0mI~X5Qd0tV7V0FKIdx9RXrQ5MYiJKkRSKcduGDcu04JtfLPOlT1VplwRQjh5pye7zoB9zzCQ467J2rGcCJ49vaXzEVKcRrlk949KM6YdmOIhGK26Ne5mnSc~lGghxO7m9PiKMDSogeuHuPJopcCJWWHw9rZtN-5HW0Sa7JQx4S35Kwxezw7nkiMNZalFIZ8kXggYTNKLodbBHRVwHSof1JVKC5WhgyrALuoLVtl-VLDWyHRvfmD9pMpNGdsRg__&amp;Key-Pair-Id=APKAIE5G5CRDK6RD3PGA</t>
+  </si>
+  <si>
+    <t>Bib</t>
+  </si>
+  <si>
+    <t>bleyer_genetic_2022</t>
+  </si>
+  <si>
+    <t>alaamery_analysis_2022</t>
+  </si>
+  <si>
+    <t>tanudisastro_australia_2021</t>
+  </si>
+  <si>
+    <t>devarajan_emerging_2022</t>
+  </si>
+  <si>
+    <t>cormican_autosomal_2019</t>
+  </si>
+  <si>
+    <t>murray_utility_2020</t>
+  </si>
+  <si>
+    <t>knoers_genetic_2022</t>
+  </si>
+  <si>
+    <t>domingo-gallego_clinical_2022</t>
+  </si>
+  <si>
+    <t>kdigo_conference_participants_genetics_2022</t>
+  </si>
+  <si>
+    <t>ottlewski_value_2019</t>
+  </si>
+  <si>
+    <t>jordan_targeted_2022</t>
+  </si>
+  <si>
+    <t>rasouly_burden_2019</t>
+  </si>
+  <si>
+    <t>elhassan_utility_2022</t>
+  </si>
+  <si>
+    <t>claus_review_2022</t>
+  </si>
+  <si>
+    <t>bullich_kidney-disease_2018</t>
+  </si>
+  <si>
+    <t>al-hamed_genetic_2016</t>
   </si>
 </sst>
 </file>
@@ -675,14 +726,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Aufgaben" displayName="Aufgaben" ref="B6:L22" totalsRowShown="0">
-  <autoFilter ref="B6:L22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Aufgaben" displayName="Aufgaben" ref="B6:M22" totalsRowShown="0">
+  <autoFilter ref="B6:M22" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Access Date" dataDxfId="7"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Publication Date" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="5"/>
@@ -693,6 +740,7 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Where to find:" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Download_link"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Type"/>
+    <tableColumn id="12" xr3:uid="{C8D3D15E-671C-4982-B471-091926564BDC}" name="Bib"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Number"/>
   </tableColumns>
   <tableStyleInfo name="Aufgaben" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -970,10 +1018,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -989,7 +1037,7 @@
     <col min="9" max="9" width="88.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
@@ -997,19 +1045,19 @@
       <c r="D1" s="3"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:12" ht="24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="24" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:12" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:12" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1020,12 +1068,12 @@
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5"/>
       <c r="D5" s="3"/>
       <c r="E5" s="23"/>
     </row>
-    <row r="6" spans="1:12" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="22.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1057,10 +1105,13 @@
         <v>76</v>
       </c>
       <c r="L6" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="6">
         <v>44977</v>
       </c>
@@ -1091,11 +1142,14 @@
       <c r="K7" t="s">
         <v>78</v>
       </c>
-      <c r="L7">
+      <c r="L7" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>44977</v>
       </c>
@@ -1126,11 +1180,14 @@
       <c r="K8" t="s">
         <v>111</v>
       </c>
-      <c r="L8">
+      <c r="L8" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <v>44977</v>
       </c>
@@ -1161,11 +1218,14 @@
       <c r="K9" t="s">
         <v>79</v>
       </c>
-      <c r="L9">
+      <c r="L9" t="s">
+        <v>118</v>
+      </c>
+      <c r="M9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
         <v>44977</v>
       </c>
@@ -1196,11 +1256,14 @@
       <c r="K10" t="s">
         <v>82</v>
       </c>
-      <c r="L10">
+      <c r="L10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6">
         <v>44977</v>
       </c>
@@ -1231,11 +1294,14 @@
       <c r="K11" t="s">
         <v>83</v>
       </c>
-      <c r="L11">
+      <c r="L11" t="s">
+        <v>119</v>
+      </c>
+      <c r="M11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6">
         <v>44977</v>
       </c>
@@ -1266,11 +1332,14 @@
       <c r="K12" t="s">
         <v>82</v>
       </c>
-      <c r="L12">
+      <c r="L12" t="s">
+        <v>120</v>
+      </c>
+      <c r="M12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6">
         <v>44977</v>
       </c>
@@ -1301,11 +1370,14 @@
       <c r="K13" t="s">
         <v>79</v>
       </c>
-      <c r="L13">
+      <c r="L13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6">
         <v>44977</v>
       </c>
@@ -1336,11 +1408,14 @@
       <c r="K14" t="s">
         <v>82</v>
       </c>
-      <c r="L14">
+      <c r="L14" t="s">
+        <v>129</v>
+      </c>
+      <c r="M14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6">
         <v>44977</v>
       </c>
@@ -1371,11 +1446,14 @@
       <c r="K15" t="s">
         <v>83</v>
       </c>
-      <c r="L15">
+      <c r="L15" t="s">
+        <v>121</v>
+      </c>
+      <c r="M15">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="6">
         <v>44977</v>
       </c>
@@ -1406,11 +1484,14 @@
       <c r="K16" t="s">
         <v>83</v>
       </c>
-      <c r="L16">
+      <c r="L16" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="6">
         <v>44977</v>
       </c>
@@ -1441,11 +1522,14 @@
       <c r="K17" t="s">
         <v>82</v>
       </c>
-      <c r="L17">
+      <c r="L17" t="s">
+        <v>130</v>
+      </c>
+      <c r="M17">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6">
         <v>44977</v>
       </c>
@@ -1476,11 +1560,14 @@
       <c r="K18" t="s">
         <v>78</v>
       </c>
-      <c r="L18">
+      <c r="L18" t="s">
+        <v>131</v>
+      </c>
+      <c r="M18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="6">
         <v>44978</v>
       </c>
@@ -1511,11 +1598,14 @@
       <c r="K19" t="s">
         <v>78</v>
       </c>
-      <c r="L19">
+      <c r="L19" t="s">
+        <v>126</v>
+      </c>
+      <c r="M19">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="6">
         <v>44978</v>
       </c>
@@ -1546,11 +1636,14 @@
       <c r="K20" t="s">
         <v>83</v>
       </c>
-      <c r="L20">
+      <c r="L20" t="s">
+        <v>132</v>
+      </c>
+      <c r="M20">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="6">
         <v>44978</v>
       </c>
@@ -1581,11 +1674,14 @@
       <c r="K21" t="s">
         <v>78</v>
       </c>
-      <c r="L21">
+      <c r="L21" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="6">
         <v>44978</v>
       </c>
@@ -1616,7 +1712,10 @@
       <c r="K22" t="s">
         <v>79</v>
       </c>
-      <c r="L22">
+      <c r="L22" t="s">
+        <v>127</v>
+      </c>
+      <c r="M22">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update lit analysis,  add comments
</commit_message>
<xml_diff>
--- a/analyses/02_Literature/data/230220_Kidney_Genes_Publication_List.xlsx
+++ b/analyses/02_Literature/data/230220_Kidney_Genes_Publication_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\kidney-genetics\analyses\02_Literature\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69406072-C255-4CF9-B8ED-B0DAC92A6931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B65EBC1-5451-46D5-87FB-75655BE7C14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>